<commit_message>
Cập nhật danh sách chức năng
</commit_message>
<xml_diff>
--- a/01.Requirement/06.DanhSachChucNang.xlsx
+++ b/01.Requirement/06.DanhSachChucNang.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Tìm nhanh tuyến xe</t>
   </si>
@@ -229,13 +229,16 @@
   </si>
   <si>
     <t>Độ ưu tiên</t>
+  </si>
+  <si>
+    <t>Hoàn thành</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +259,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -388,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -399,56 +407,68 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -465,16 +485,19 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -493,21 +516,29 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -619,6 +650,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -626,47 +666,38 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -674,13 +705,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:D48" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A3:D48"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="STT" dataDxfId="4"/>
-    <tableColumn id="2" name="Tên chức năng" dataDxfId="3"/>
-    <tableColumn id="3" name="Usecase" dataDxfId="2"/>
-    <tableColumn id="4" name="Độ ưu tiên" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E48" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A3:E48">
+    <filterColumn colId="3"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="STT" dataDxfId="5"/>
+    <tableColumn id="2" name="Tên chức năng" dataDxfId="4"/>
+    <tableColumn id="3" name="Usecase" dataDxfId="3"/>
+    <tableColumn id="5" name="Độ ưu tiên" dataDxfId="1"/>
+    <tableColumn id="4" name="Hoàn thành" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -971,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,713 +1016,776 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="33.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="19.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="10" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="19" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="8">
+      <c r="E3" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="E4" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="8">
+    <row r="5" spans="1:8">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1.2</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
+      <c r="E5" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="8">
+    <row r="6" spans="1:8">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>1.3</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="E6" s="21"/>
+      <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="8">
+    <row r="7" spans="1:8">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>1.4</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="E7" s="21"/>
+      <c r="G7" s="1">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="8">
+    <row r="8" spans="1:8">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>1.5</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>6</v>
       </c>
-      <c r="F8" s="1">
+      <c r="E8" s="21"/>
+      <c r="G8" s="1">
         <v>4</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="8">
+    <row r="9" spans="1:8">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>2.1</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="1">
+      <c r="E9" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="G9" s="1">
         <v>5</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="8">
+    <row r="10" spans="1:8">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="8">
+      <c r="E10" s="21">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="8">
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>2.4</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="8">
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>2.5</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="8">
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7">
         <v>11</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>3.1</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="8">
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7">
         <v>12</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>3.2</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="8">
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7">
         <v>13</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>3.3</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="8">
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="7">
         <v>14</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>3.4</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="8">
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="7">
         <v>15</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="8">
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="7">
         <v>16</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>4.2</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="8">
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="7">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>4.3</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="8">
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="7">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="8">
+      <c r="E21" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="7">
         <v>19</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>4.5</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="8">
+      <c r="E22" s="21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="7">
         <v>20</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="8">
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7">
         <v>21</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>4.7</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="8">
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="7">
         <v>22</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>4.8</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="8">
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="7">
         <v>23</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="8">
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="7">
         <v>24</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="8">
+      <c r="E27" s="21"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="7">
         <v>25</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>4.1100000000000003</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="8">
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="7">
         <v>26</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>4.12</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="8">
+      <c r="E29" s="21"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="7">
         <v>27</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>4.13</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="8">
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="7">
         <v>28</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="8">
+      <c r="E31" s="21"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="7">
         <v>29</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="8">
+      <c r="E32" s="21"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="7">
         <v>30</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>4.16</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="8">
+      <c r="E33" s="21"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="7">
         <v>31</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="8">
+      <c r="E34" s="21"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7">
         <v>32</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="8">
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7">
         <v>33</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="8">
+      <c r="E36" s="21"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="7">
         <v>34</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="8">
+      <c r="E37" s="21"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="7">
         <v>35</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="8">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="8">
+      <c r="E38" s="21"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="7">
         <v>36</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="8">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="8">
+      <c r="E39" s="21"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="7">
         <v>37</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="8">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="8">
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7">
         <v>38</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="8">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="8">
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="7">
         <v>39</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="8">
+      <c r="E42" s="21"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="7">
         <v>40</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="8">
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="7">
         <v>41</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="8">
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="7">
         <v>42</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="8">
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="7">
         <v>43</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="8">
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="7">
         <v>44</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="8">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="14">
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="13">
         <v>45</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="16">
         <v>13</v>
       </c>
+      <c r="E48" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:C48">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"left($C$4, 1) = '1'"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Thay đổi dữ liệu
</commit_message>
<xml_diff>
--- a/01.Requirement/06.DanhSachChucNang.xlsx
+++ b/01.Requirement/06.DanhSachChucNang.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>Tìm nhanh tuyến xe</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>Nhi, Huy</t>
+  </si>
+  <si>
+    <t>Tú, Nhi</t>
+  </si>
+  <si>
+    <t>Huy, Kiều</t>
+  </si>
+  <si>
+    <t>Lê, Kiều</t>
   </si>
 </sst>
 </file>
@@ -476,11 +485,11 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1063,22 +1072,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
     </row>
@@ -1098,7 +1107,7 @@
       <c r="E3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1164,7 +1173,12 @@
       <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
@@ -1206,7 +1220,12 @@
       <c r="D8" s="8">
         <v>6</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="20">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="G8" s="1">
         <v>4</v>
       </c>
@@ -1600,7 +1619,7 @@
       </c>
       <c r="E32" s="20"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" s="7">
         <v>30</v>
       </c>
@@ -1615,7 +1634,7 @@
       </c>
       <c r="E33" s="20"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" s="7">
         <v>31</v>
       </c>
@@ -1628,9 +1647,14 @@
       <c r="D34" s="8">
         <v>2</v>
       </c>
-      <c r="E34" s="20"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="E34" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -1645,7 +1669,7 @@
       </c>
       <c r="E35" s="20"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" s="7">
         <v>33</v>
       </c>
@@ -1660,7 +1684,7 @@
       </c>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -1675,7 +1699,7 @@
       </c>
       <c r="E37" s="20"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38" s="7">
         <v>35</v>
       </c>
@@ -1690,7 +1714,7 @@
       </c>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" s="7">
         <v>36</v>
       </c>
@@ -1705,7 +1729,7 @@
       </c>
       <c r="E39" s="20"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:6">
       <c r="A40" s="7">
         <v>37</v>
       </c>
@@ -1720,7 +1744,7 @@
       </c>
       <c r="E40" s="20"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:6">
       <c r="A41" s="7">
         <v>38</v>
       </c>
@@ -1735,7 +1759,7 @@
       </c>
       <c r="E41" s="20"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:6">
       <c r="A42" s="7">
         <v>39</v>
       </c>
@@ -1750,7 +1774,7 @@
       </c>
       <c r="E42" s="20"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:6">
       <c r="A43" s="7">
         <v>40</v>
       </c>
@@ -1765,7 +1789,7 @@
       </c>
       <c r="E43" s="20"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:6">
       <c r="A44" s="7">
         <v>41</v>
       </c>
@@ -1780,7 +1804,7 @@
       </c>
       <c r="E44" s="20"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:6">
       <c r="A45" s="7">
         <v>42</v>
       </c>
@@ -1795,7 +1819,7 @@
       </c>
       <c r="E45" s="20"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:6">
       <c r="A46" s="7">
         <v>43</v>
       </c>
@@ -1810,7 +1834,7 @@
       </c>
       <c r="E46" s="20"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:6">
       <c r="A47" s="7">
         <v>44</v>
       </c>
@@ -1825,7 +1849,7 @@
       </c>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:6">
       <c r="A48" s="13">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Chỉnh sửa store cho phù hợp với dữ liệu mới bảng PHAN_HOI_KHACH_HANG Thêm chức năng duyệt phản hồi
</commit_message>
<xml_diff>
--- a/01.Requirement/06.DanhSachChucNang.xlsx
+++ b/01.Requirement/06.DanhSachChucNang.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
   <si>
     <t>Tìm nhanh tuyến xe</t>
   </si>
@@ -506,24 +506,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -765,24 +758,31 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:F48" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:F48" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A3:F48">
     <filterColumn colId="3"/>
     <filterColumn colId="5"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="STT" dataDxfId="6"/>
-    <tableColumn id="2" name="Tên chức năng" dataDxfId="5"/>
-    <tableColumn id="3" name="Usecase" dataDxfId="4"/>
-    <tableColumn id="5" name="Độ ưu tiên" dataDxfId="3"/>
-    <tableColumn id="4" name="Hoàn thành" dataDxfId="2"/>
-    <tableColumn id="6" name="Phân công" dataDxfId="1"/>
+    <tableColumn id="1" name="STT" dataDxfId="5"/>
+    <tableColumn id="2" name="Tên chức năng" dataDxfId="4"/>
+    <tableColumn id="3" name="Usecase" dataDxfId="3"/>
+    <tableColumn id="5" name="Độ ưu tiên" dataDxfId="2"/>
+    <tableColumn id="4" name="Hoàn thành" dataDxfId="1"/>
+    <tableColumn id="6" name="Phân công" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1093,22 +1093,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
     </row>
@@ -1339,9 +1339,8 @@
         <v>3</v>
       </c>
       <c r="E12" s="20"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="1" t="s">
-        <v>75</v>
+      <c r="F12" s="23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1856,7 +1855,12 @@
       <c r="D42" s="8">
         <v>6</v>
       </c>
-      <c r="E42" s="20"/>
+      <c r="E42" s="20">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="G42" s="1" t="s">
         <v>74</v>
       </c>
@@ -1874,7 +1878,9 @@
       <c r="D43" s="8">
         <v>6</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="20">
+        <v>0.5</v>
+      </c>
       <c r="G43" s="1" t="s">
         <v>74</v>
       </c>
@@ -1965,7 +1971,7 @@
     <mergeCell ref="A1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:C48">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"left($C$4, 1) = '1'"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Chỉnh sửa store select nhân viên Cập nhật danh sách chức năng Thêm validator giá vé cho wucThemTuyen
</commit_message>
<xml_diff>
--- a/01.Requirement/06.DanhSachChucNang.xlsx
+++ b/01.Requirement/06.DanhSachChucNang.xlsx
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1338,7 +1338,9 @@
       <c r="D12" s="8">
         <v>3</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="20">
+        <v>0.9</v>
+      </c>
       <c r="F12" s="23" t="s">
         <v>80</v>
       </c>
@@ -1553,8 +1555,10 @@
       <c r="D24" s="8">
         <v>8</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="G24" s="1" t="s">
+      <c r="E24" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1571,8 +1575,10 @@
       <c r="D25" s="8">
         <v>8</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="G25" s="1" t="s">
+      <c r="E25" s="20">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Yêu cầu của Thầy
</commit_message>
<xml_diff>
--- a/01.Requirement/06.DanhSachChucNang.xlsx
+++ b/01.Requirement/06.DanhSachChucNang.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
   <si>
     <t>Tìm nhanh tuyến xe</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Nhi</t>
+  </si>
+  <si>
+    <t>Bùi, Kiều</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1625,9 +1628,11 @@
       <c r="D28" s="8">
         <v>9</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="G28" s="1" t="s">
-        <v>81</v>
+      <c r="E28" s="20">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1643,7 +1648,12 @@
       <c r="D29" s="8">
         <v>9</v>
       </c>
-      <c r="E29" s="20"/>
+      <c r="E29" s="20">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="7">
@@ -1658,7 +1668,12 @@
       <c r="D30" s="8">
         <v>9</v>
       </c>
-      <c r="E30" s="20"/>
+      <c r="E30" s="20">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="7">
@@ -1673,7 +1688,12 @@
       <c r="D31" s="8">
         <v>9</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="20">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="7">
@@ -1904,7 +1924,9 @@
       <c r="D44" s="8">
         <v>5</v>
       </c>
-      <c r="E44" s="20"/>
+      <c r="E44" s="20">
+        <v>1</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>83</v>
       </c>
@@ -1922,7 +1944,9 @@
       <c r="D45" s="8">
         <v>5</v>
       </c>
-      <c r="E45" s="20"/>
+      <c r="E45" s="20">
+        <v>1</v>
+      </c>
       <c r="G45" s="1" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật DS chức năng
</commit_message>
<xml_diff>
--- a/01.Requirement/06.DanhSachChucNang.xlsx
+++ b/01.Requirement/06.DanhSachChucNang.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
   <si>
     <t>Tìm nhanh tuyến xe</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>Bùi, Kiều</t>
+  </si>
+  <si>
+    <t>Nhi Huy</t>
+  </si>
+  <si>
+    <t>Huy Tú</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1481,6 +1487,9 @@
         <v>4</v>
       </c>
       <c r="E20" s="20"/>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="G20" s="1" t="s">
         <v>81</v>
       </c>
@@ -1599,6 +1608,9 @@
         <v>8</v>
       </c>
       <c r="E26" s="20"/>
+      <c r="F26" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="7">
@@ -1614,6 +1626,9 @@
         <v>8</v>
       </c>
       <c r="E27" s="20"/>
+      <c r="F27" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="7">

</xml_diff>